<commit_message>
finish up power generation exercise
</commit_message>
<xml_diff>
--- a/power_generation/data.xlsx
+++ b/power_generation/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\REPOSITORIES\optimization\power_generation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9AF0382-C676-4D71-BDDC-B5A25B2922AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A2C81A-AFFC-4346-B5D6-D7935F386336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{18B9DBA3-F265-4658-BC94-56B3DCA99A89}"/>
   </bookViews>
@@ -401,7 +401,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE44DB6-3585-45CE-B386-C5422EB4D2DB}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C2:C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -454,7 +456,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="C5">
         <v>50</v>

</xml_diff>